<commit_message>
Agregado de retrazo forzado para mejorar output
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120704/Performance del procesador.xlsx
+++ b/Documentacion/drafts/20120704/Performance del procesador.xlsx
@@ -111,9 +111,6 @@
     <t>[200T-&gt;P]</t>
   </si>
   <si>
-    <t>[1000T-&gt;P]</t>
-  </si>
-  <si>
     <t>Input(tareas/ms)</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>TestDePerformanceEnOptimunConSaturacionKnittle</t>
+  </si>
+  <si>
+    <t>[2000T-&gt;P]</t>
   </si>
 </sst>
 </file>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +543,7 @@
     </row>
     <row r="5" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
@@ -554,10 +554,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
@@ -574,25 +574,25 @@
         <v>13</v>
       </c>
       <c r="E7">
-        <v>10000</v>
+        <v>10016</v>
       </c>
       <c r="F7" s="1">
-        <v>524.06370000000004</v>
+        <v>526.59325079872201</v>
       </c>
       <c r="G7" s="1">
-        <v>524.06359999999995</v>
+        <v>526.59305111821004</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" ref="H7:H13" si="0">G7/F7</f>
-        <v>0.99999980918350173</v>
+        <v>0.99999962080692895</v>
       </c>
       <c r="I7" s="5">
         <f>F7*1000</f>
-        <v>524063.7</v>
+        <v>526593.25079872203</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" ref="J7:J50" si="1">G7*1000</f>
-        <v>524063.6</v>
+        <v>526593.05111821007</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
@@ -603,22 +603,22 @@
         <v>10000</v>
       </c>
       <c r="F8" s="1">
-        <v>486.70280000000002</v>
+        <v>480.5324</v>
       </c>
       <c r="G8" s="1">
-        <v>486.70209999999997</v>
+        <v>480.53219999999999</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999856175062063</v>
+        <v>0.99999958379497411</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" ref="I8:I13" si="2">F8*1000</f>
-        <v>486702.80000000005</v>
+        <v>480532.4</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="1"/>
-        <v>486702.1</v>
+        <v>480532.2</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
@@ -629,22 +629,22 @@
         <v>10000</v>
       </c>
       <c r="F9" s="1">
-        <v>497.68799999999999</v>
+        <v>481.23910000000001</v>
       </c>
       <c r="G9" s="1">
-        <v>497.68599999999998</v>
+        <v>481.2389</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999598141807722</v>
+        <v>0.99999958440617143</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="2"/>
-        <v>497688</v>
+        <v>481239.10000000003</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>497686</v>
+        <v>481238.9</v>
       </c>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.25">
@@ -652,25 +652,25 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>10000</v>
+        <v>10016</v>
       </c>
       <c r="F10" s="1">
-        <v>493.91469999999998</v>
+        <v>482.11711261980798</v>
       </c>
       <c r="G10" s="1">
-        <v>493.91449999999998</v>
+        <v>482.11691293929698</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>0.9999995950717806</v>
+        <v>0.9999995858257138</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="2"/>
-        <v>493914.69999999995</v>
+        <v>482117.112619808</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="1"/>
-        <v>493914.5</v>
+        <v>482116.91293929698</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
@@ -681,22 +681,22 @@
         <v>10000</v>
       </c>
       <c r="F11" s="1">
-        <v>502.13510000000002</v>
+        <v>469.99029999999999</v>
       </c>
       <c r="G11" s="1">
-        <v>502.13499999999999</v>
+        <v>469.99020000000002</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999980085040852</v>
+        <v>0.99999978722965144</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="2"/>
-        <v>502135.10000000003</v>
+        <v>469990.3</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="1"/>
-        <v>502135</v>
+        <v>469990.2</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
@@ -707,22 +707,22 @@
         <v>10015</v>
       </c>
       <c r="F12" s="1">
-        <v>517.49216175736399</v>
+        <v>465.40199700449301</v>
       </c>
       <c r="G12" s="1">
-        <v>517.49086370444297</v>
+        <v>465.40179730404299</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999749164718432</v>
+        <v>0.99999957090762115</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="2"/>
-        <v>517492.161757364</v>
+        <v>465401.99700449302</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="1"/>
-        <v>517490.86370444298</v>
+        <v>465401.79730404296</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
@@ -733,48 +733,48 @@
         <v>10047</v>
       </c>
       <c r="F13" s="1">
-        <v>506.23509505324898</v>
+        <v>476.159948243256</v>
       </c>
       <c r="G13" s="1">
-        <v>506.23429879565998</v>
+        <v>476.15865432467399</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999842709919406</v>
+        <v>0.99999728259676868</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="2"/>
-        <v>506235.09505324898</v>
+        <v>476159.94824325602</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="1"/>
-        <v>506234.29879565997</v>
+        <v>476158.65432467399</v>
       </c>
     </row>
     <row r="14" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E14">
-        <v>10500</v>
+        <v>10547</v>
       </c>
       <c r="F14" s="1">
-        <v>453.56104761904697</v>
+        <v>465.42438608135001</v>
       </c>
       <c r="G14" s="1">
-        <v>453.56038095238</v>
+        <v>465.42410164027598</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14" si="3">G14/F14</f>
-        <v>0.99999853015008566</v>
+        <v>0.99999938885653061</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" ref="I14" si="4">F14*1000</f>
-        <v>453561.04761904699</v>
+        <v>465424.38608135004</v>
       </c>
       <c r="J14" s="6">
         <f t="shared" ref="J14" si="5">G14*1000</f>
-        <v>453560.38095238002</v>
+        <v>465424.10164027597</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
     </row>
     <row r="16" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
@@ -799,10 +799,10 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
         <v>21</v>
-      </c>
-      <c r="G17" t="s">
-        <v>22</v>
       </c>
       <c r="H17" t="s">
         <v>5</v>
@@ -819,25 +819,25 @@
         <v>13</v>
       </c>
       <c r="E18">
-        <v>12531</v>
+        <v>10000</v>
       </c>
       <c r="F18" s="1">
-        <v>302.90192323038798</v>
+        <v>153.9769</v>
       </c>
       <c r="G18" s="1">
-        <v>72.792035751336599</v>
+        <v>153.96129999999999</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" ref="H18:H25" si="6">G18/F18</f>
-        <v>0.24031552845562751</v>
+        <v>0.99989868610161647</v>
       </c>
       <c r="I18" s="7">
         <f>F18*1000</f>
-        <v>302901.92323038797</v>
+        <v>153976.9</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" ref="J18:J25" si="7">G18*1000</f>
-        <v>72792.035751336603</v>
+        <v>153961.29999999999</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
@@ -845,25 +845,25 @@
         <v>14</v>
       </c>
       <c r="E19">
-        <v>10046</v>
+        <v>10000</v>
       </c>
       <c r="F19" s="1">
-        <v>441.92414891499101</v>
+        <v>157.39109999999999</v>
       </c>
       <c r="G19" s="1">
-        <v>76.038025084610794</v>
+        <v>157.38749999999999</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="6"/>
-        <v>0.17206125818491433</v>
+        <v>0.99997712704212627</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" ref="I19:I25" si="8">F19*1000</f>
-        <v>441924.148914991</v>
+        <v>157391.1</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="7"/>
-        <v>76038.025084610796</v>
+        <v>157387.5</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
@@ -871,25 +871,25 @@
         <v>15</v>
       </c>
       <c r="E20">
-        <v>10532</v>
+        <v>10000</v>
       </c>
       <c r="F20" s="1">
-        <v>431.34969616407102</v>
+        <v>157.43100000000001</v>
       </c>
       <c r="G20" s="1">
-        <v>54.108051652107797</v>
+        <v>157.42910000000001</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="6"/>
-        <v>0.12543894694555877</v>
+        <v>0.99998793122066176</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="8"/>
-        <v>431349.69616407104</v>
+        <v>157431</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="7"/>
-        <v>54108.051652107795</v>
+        <v>157429.1</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
@@ -897,25 +897,25 @@
         <v>16</v>
       </c>
       <c r="E21">
-        <v>10203</v>
+        <v>10031</v>
       </c>
       <c r="F21" s="1">
-        <v>421.43732235616898</v>
+        <v>154.53215033396401</v>
       </c>
       <c r="G21" s="1">
-        <v>34.810055865921697</v>
+        <v>154.501844282723</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="6"/>
-        <v>8.2598417414257164E-2</v>
+        <v>0.99980388513862317</v>
       </c>
       <c r="I21" s="7">
         <f t="shared" si="8"/>
-        <v>421437.322356169</v>
+        <v>154532.150333964</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="7"/>
-        <v>34810.055865921699</v>
+        <v>154501.844282723</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
@@ -923,25 +923,25 @@
         <v>18</v>
       </c>
       <c r="E22">
-        <v>10125</v>
+        <v>10016</v>
       </c>
       <c r="F22" s="1">
-        <v>467.45165432098702</v>
+        <v>156.50938498402499</v>
       </c>
       <c r="G22" s="1">
-        <v>57.209481481481397</v>
+        <v>156.47893370606999</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="6"/>
-        <v>0.12238587873773385</v>
+        <v>0.99980543481173278</v>
       </c>
       <c r="I22" s="5">
         <f t="shared" si="8"/>
-        <v>467451.654320987</v>
+        <v>156509.384984025</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="7"/>
-        <v>57209.481481481394</v>
+        <v>156478.93370607001</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
@@ -949,25 +949,25 @@
         <v>17</v>
       </c>
       <c r="E23">
-        <v>10031</v>
+        <v>10093</v>
       </c>
       <c r="F23" s="1">
-        <v>466.34652577011201</v>
+        <v>152.08391954820101</v>
       </c>
       <c r="G23" s="1">
-        <v>61.019938191606002</v>
+        <v>152.053799663132</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="6"/>
-        <v>0.13084677341776982</v>
+        <v>0.9998019522040299</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" si="8"/>
-        <v>466346.525770112</v>
+        <v>152083.919548201</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="7"/>
-        <v>61019.938191606001</v>
+        <v>152053.799663132</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
@@ -975,51 +975,51 @@
         <v>19</v>
       </c>
       <c r="E24">
-        <v>12187</v>
+        <v>10563</v>
       </c>
       <c r="F24" s="1">
-        <v>379.42340198572202</v>
+        <v>153.37707090788601</v>
       </c>
       <c r="G24" s="1">
-        <v>41.822269631574599</v>
+        <v>153.348196535075</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="6"/>
-        <v>0.11022585695214551</v>
+        <v>0.9998117425724713</v>
       </c>
       <c r="I24" s="7">
         <f t="shared" si="8"/>
-        <v>379423.40198572201</v>
+        <v>153377.07090788599</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="7"/>
-        <v>41822.2696315746</v>
+        <v>153348.196535075</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E25">
-        <v>69531</v>
+        <v>16391</v>
       </c>
       <c r="F25" s="1">
-        <v>78.606319483395893</v>
+        <v>144.614666585321</v>
       </c>
       <c r="G25" s="1">
-        <v>22.223382376206199</v>
+        <v>144.59978036727401</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="6"/>
-        <v>0.28271750315062738</v>
+        <v>0.999897062874752</v>
       </c>
       <c r="I25" s="6">
         <f t="shared" si="8"/>
-        <v>78606.319483395899</v>
+        <v>144614.66658532101</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" si="7"/>
-        <v>22223.382376206198</v>
+        <v>144599.78036727401</v>
       </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
@@ -1044,10 +1044,10 @@
         <v>4</v>
       </c>
       <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
         <v>21</v>
-      </c>
-      <c r="G28" t="s">
-        <v>22</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E36">
         <v>11422</v>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -1291,10 +1291,10 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" t="s">
         <v>21</v>
-      </c>
-      <c r="G39" t="s">
-        <v>22</v>
       </c>
       <c r="H39" t="s">
         <v>5</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E47">
         <v>28281</v>

</xml_diff>

<commit_message>
Metricas opcionales en el procesador
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120704/Performance del procesador.xlsx
+++ b/Documentacion/drafts/20120704/Performance del procesador.xlsx
@@ -510,7 +510,7 @@
   <dimension ref="D2:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,25 +574,25 @@
         <v>13</v>
       </c>
       <c r="E7">
-        <v>10016</v>
+        <v>10000</v>
       </c>
       <c r="F7" s="1">
-        <v>526.59325079872201</v>
+        <v>509.79059999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>526.59305111821004</v>
+        <v>509.7903</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" ref="H7:H13" si="0">G7/F7</f>
-        <v>0.99999962080692895</v>
-      </c>
-      <c r="I7" s="5">
+        <v>0.99999941152308425</v>
+      </c>
+      <c r="I7" s="7">
         <f>F7*1000</f>
-        <v>526593.25079872203</v>
-      </c>
-      <c r="J7" s="5">
+        <v>509790.6</v>
+      </c>
+      <c r="J7" s="7">
         <f t="shared" ref="J7:J50" si="1">G7*1000</f>
-        <v>526593.05111821007</v>
+        <v>509790.3</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
@@ -603,22 +603,22 @@
         <v>10000</v>
       </c>
       <c r="F8" s="1">
-        <v>480.5324</v>
+        <v>511.88979999999998</v>
       </c>
       <c r="G8" s="1">
-        <v>480.53219999999999</v>
+        <v>511.88889999999998</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999958379497411</v>
-      </c>
-      <c r="I8" s="7">
+        <v>0.99999824180907693</v>
+      </c>
+      <c r="I8" s="5">
         <f t="shared" ref="I8:I13" si="2">F8*1000</f>
-        <v>480532.4</v>
-      </c>
-      <c r="J8" s="7">
+        <v>511889.8</v>
+      </c>
+      <c r="J8" s="5">
         <f t="shared" si="1"/>
-        <v>480532.2</v>
+        <v>511888.89999999997</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
@@ -629,22 +629,22 @@
         <v>10000</v>
       </c>
       <c r="F9" s="1">
-        <v>481.23910000000001</v>
+        <v>484.18310000000002</v>
       </c>
       <c r="G9" s="1">
-        <v>481.2389</v>
+        <v>484.18299999999999</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999958440617143</v>
+        <v>0.99999979346656243</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="2"/>
-        <v>481239.10000000003</v>
+        <v>484183.10000000003</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>481238.9</v>
+        <v>484183</v>
       </c>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.25">
@@ -655,22 +655,22 @@
         <v>10016</v>
       </c>
       <c r="F10" s="1">
-        <v>482.11711261980798</v>
+        <v>469.22873402555899</v>
       </c>
       <c r="G10" s="1">
-        <v>482.11691293929698</v>
+        <v>469.22863418530301</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>0.9999995858257138</v>
+        <v>0.99999978722476113</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="2"/>
-        <v>482117.112619808</v>
+        <v>469228.73402555898</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="1"/>
-        <v>482116.91293929698</v>
+        <v>469228.634185303</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
@@ -681,22 +681,22 @@
         <v>10000</v>
       </c>
       <c r="F11" s="1">
-        <v>469.99029999999999</v>
+        <v>479.036</v>
       </c>
       <c r="G11" s="1">
-        <v>469.99020000000002</v>
+        <v>479.03590000000003</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999978722965144</v>
+        <v>0.999999791247422</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="2"/>
-        <v>469990.3</v>
+        <v>479036</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="1"/>
-        <v>469990.2</v>
+        <v>479035.9</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
@@ -704,25 +704,25 @@
         <v>17</v>
       </c>
       <c r="E12">
-        <v>10015</v>
+        <v>10016</v>
       </c>
       <c r="F12" s="1">
-        <v>465.40199700449301</v>
+        <v>477.907348242811</v>
       </c>
       <c r="G12" s="1">
-        <v>465.40179730404299</v>
+        <v>477.90634984025502</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999957090762115</v>
+        <v>0.99999791088678658</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="2"/>
-        <v>465401.99700449302</v>
+        <v>477907.34824281099</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="1"/>
-        <v>465401.79730404296</v>
+        <v>477906.34984025505</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
@@ -730,25 +730,25 @@
         <v>19</v>
       </c>
       <c r="E13">
-        <v>10047</v>
+        <v>10046</v>
       </c>
       <c r="F13" s="1">
-        <v>476.159948243256</v>
+        <v>479.30708739796898</v>
       </c>
       <c r="G13" s="1">
-        <v>476.15865432467399</v>
+        <v>479.30688831375602</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999728259676868</v>
+        <v>0.99999958464162497</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="2"/>
-        <v>476159.94824325602</v>
+        <v>479307.08739796898</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="1"/>
-        <v>476158.65432467399</v>
+        <v>479306.88831375603</v>
       </c>
     </row>
     <row r="14" spans="4:10" x14ac:dyDescent="0.25">
@@ -756,25 +756,25 @@
         <v>26</v>
       </c>
       <c r="E14">
-        <v>10547</v>
+        <v>10516</v>
       </c>
       <c r="F14" s="1">
-        <v>465.42438608135001</v>
+        <v>454.49153670597099</v>
       </c>
       <c r="G14" s="1">
-        <v>465.42410164027598</v>
+        <v>454.49144161278002</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14" si="3">G14/F14</f>
-        <v>0.99999938885653061</v>
+        <v>0.99999979077016121</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" ref="I14" si="4">F14*1000</f>
-        <v>465424.38608135004</v>
+        <v>454491.536705971</v>
       </c>
       <c r="J14" s="6">
         <f t="shared" ref="J14" si="5">G14*1000</f>
-        <v>465424.10164027597</v>
+        <v>454491.44161278004</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.25">
@@ -822,22 +822,22 @@
         <v>10000</v>
       </c>
       <c r="F18" s="1">
-        <v>153.9769</v>
+        <v>155.8672</v>
       </c>
       <c r="G18" s="1">
-        <v>153.96129999999999</v>
+        <v>155.8578</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" ref="H18:H25" si="6">G18/F18</f>
-        <v>0.99989868610161647</v>
+        <v>0.99993969225083923</v>
       </c>
       <c r="I18" s="7">
         <f>F18*1000</f>
-        <v>153976.9</v>
+        <v>155867.19999999998</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" ref="J18:J25" si="7">G18*1000</f>
-        <v>153961.29999999999</v>
+        <v>155857.79999999999</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
@@ -848,22 +848,22 @@
         <v>10000</v>
       </c>
       <c r="F19" s="1">
-        <v>157.39109999999999</v>
+        <v>155.7311</v>
       </c>
       <c r="G19" s="1">
-        <v>157.38749999999999</v>
+        <v>155.73089999999999</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="6"/>
-        <v>0.99997712704212627</v>
+        <v>0.99999871573500732</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" ref="I19:I25" si="8">F19*1000</f>
-        <v>157391.1</v>
-      </c>
-      <c r="J19" s="5">
+        <v>155731.1</v>
+      </c>
+      <c r="J19" s="7">
         <f t="shared" si="7"/>
-        <v>157387.5</v>
+        <v>155730.9</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
@@ -874,22 +874,22 @@
         <v>10000</v>
       </c>
       <c r="F20" s="1">
-        <v>157.43100000000001</v>
+        <v>157.5197</v>
       </c>
       <c r="G20" s="1">
-        <v>157.42910000000001</v>
+        <v>157.5179</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="6"/>
-        <v>0.99998793122066176</v>
+        <v>0.99998857285787113</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="8"/>
-        <v>157431</v>
+        <v>157519.70000000001</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="7"/>
-        <v>157429.1</v>
+        <v>157517.9</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
@@ -900,22 +900,22 @@
         <v>10031</v>
       </c>
       <c r="F21" s="1">
-        <v>154.53215033396401</v>
+        <v>160.064599740803</v>
       </c>
       <c r="G21" s="1">
-        <v>154.501844282723</v>
+        <v>160.03977669225401</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="6"/>
-        <v>0.99980388513862317</v>
-      </c>
-      <c r="I21" s="7">
+        <v>0.99984491856044877</v>
+      </c>
+      <c r="I21" s="5">
         <f t="shared" si="8"/>
-        <v>154532.150333964</v>
-      </c>
-      <c r="J21" s="7">
+        <v>160064.59974080301</v>
+      </c>
+      <c r="J21" s="5">
         <f t="shared" si="7"/>
-        <v>154501.844282723</v>
+        <v>160039.776692254</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
@@ -923,25 +923,25 @@
         <v>18</v>
       </c>
       <c r="E22">
-        <v>10016</v>
+        <v>10031</v>
       </c>
       <c r="F22" s="1">
-        <v>156.50938498402499</v>
+        <v>158.68407935400199</v>
       </c>
       <c r="G22" s="1">
-        <v>156.47893370606999</v>
+        <v>158.664041471438</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="6"/>
-        <v>0.99980543481173278</v>
-      </c>
-      <c r="I22" s="5">
+        <v>0.99987372468211322</v>
+      </c>
+      <c r="I22" s="7">
         <f t="shared" si="8"/>
-        <v>156509.384984025</v>
+        <v>158684.07935400199</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="7"/>
-        <v>156478.93370607001</v>
+        <v>158664.04147143799</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
@@ -949,25 +949,25 @@
         <v>17</v>
       </c>
       <c r="E23">
-        <v>10093</v>
+        <v>10047</v>
       </c>
       <c r="F23" s="1">
-        <v>152.08391954820101</v>
+        <v>157.733452771971</v>
       </c>
       <c r="G23" s="1">
-        <v>152.053799663132</v>
+        <v>157.706877674927</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="6"/>
-        <v>0.9998019522040299</v>
+        <v>0.99983151895443245</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" si="8"/>
-        <v>152083.919548201</v>
+        <v>157733.452771971</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="7"/>
-        <v>152053.799663132</v>
+        <v>157706.877674927</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
@@ -975,25 +975,25 @@
         <v>19</v>
       </c>
       <c r="E24">
-        <v>10563</v>
+        <v>10656</v>
       </c>
       <c r="F24" s="1">
-        <v>153.37707090788601</v>
+        <v>155.115709459459</v>
       </c>
       <c r="G24" s="1">
-        <v>153.348196535075</v>
+        <v>155.09168543543501</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="6"/>
-        <v>0.9998117425724713</v>
+        <v>0.9998451219150678</v>
       </c>
       <c r="I24" s="7">
         <f t="shared" si="8"/>
-        <v>153377.07090788599</v>
+        <v>155115.709459459</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="7"/>
-        <v>153348.196535075</v>
+        <v>155091.68543543501</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
@@ -1001,25 +1001,25 @@
         <v>26</v>
       </c>
       <c r="E25">
-        <v>16391</v>
+        <v>13984</v>
       </c>
       <c r="F25" s="1">
-        <v>144.614666585321</v>
+        <v>144.775886727688</v>
       </c>
       <c r="G25" s="1">
-        <v>144.59978036727401</v>
+        <v>144.77338386727601</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="6"/>
-        <v>0.999897062874752</v>
+        <v>0.99998271217349399</v>
       </c>
       <c r="I25" s="6">
         <f t="shared" si="8"/>
-        <v>144614.66658532101</v>
+        <v>144775.88672768799</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" si="7"/>
-        <v>144599.78036727401</v>
+        <v>144773.38386727602</v>
       </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bouncer en el knittle supera a executor
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120704/Performance del procesador.xlsx
+++ b/Documentacion/drafts/20120704/Performance del procesador.xlsx
@@ -510,7 +510,7 @@
   <dimension ref="D2:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,25 +574,25 @@
         <v>13</v>
       </c>
       <c r="E7">
-        <v>10000</v>
+        <v>10016</v>
       </c>
       <c r="F7" s="1">
-        <v>509.79059999999998</v>
+        <v>526.24940095846603</v>
       </c>
       <c r="G7" s="1">
-        <v>509.7903</v>
+        <v>526.24790335463194</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" ref="H7:H13" si="0">G7/F7</f>
-        <v>0.99999941152308425</v>
+        <v>0.99999715419375046</v>
       </c>
       <c r="I7" s="7">
         <f>F7*1000</f>
-        <v>509790.6</v>
+        <v>526249.40095846599</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" ref="J7:J50" si="1">G7*1000</f>
-        <v>509790.3</v>
+        <v>526247.90335463197</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
@@ -603,22 +603,22 @@
         <v>10000</v>
       </c>
       <c r="F8" s="1">
-        <v>511.88979999999998</v>
+        <v>476.42959999999999</v>
       </c>
       <c r="G8" s="1">
-        <v>511.88889999999998</v>
+        <v>476.42910000000001</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999824180907693</v>
-      </c>
-      <c r="I8" s="5">
+        <v>0.99999895052700338</v>
+      </c>
+      <c r="I8" s="7">
         <f t="shared" ref="I8:I13" si="2">F8*1000</f>
-        <v>511889.8</v>
-      </c>
-      <c r="J8" s="5">
+        <v>476429.6</v>
+      </c>
+      <c r="J8" s="7">
         <f t="shared" si="1"/>
-        <v>511888.89999999997</v>
+        <v>476429.1</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
@@ -629,22 +629,22 @@
         <v>10000</v>
       </c>
       <c r="F9" s="1">
-        <v>484.18310000000002</v>
+        <v>460.37329999999997</v>
       </c>
       <c r="G9" s="1">
-        <v>484.18299999999999</v>
+        <v>460.3732</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999979346656243</v>
+        <v>0.99999978278497037</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="2"/>
-        <v>484183.10000000003</v>
+        <v>460373.3</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>484183</v>
+        <v>460373.2</v>
       </c>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.25">
@@ -655,22 +655,22 @@
         <v>10016</v>
       </c>
       <c r="F10" s="1">
-        <v>469.22873402555899</v>
+        <v>487.64327076677301</v>
       </c>
       <c r="G10" s="1">
-        <v>469.22863418530301</v>
+        <v>487.64327076677301</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999978722476113</v>
+        <v>1</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="2"/>
-        <v>469228.73402555898</v>
+        <v>487643.27076677303</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="1"/>
-        <v>469228.634185303</v>
+        <v>487643.27076677303</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
@@ -681,22 +681,22 @@
         <v>10000</v>
       </c>
       <c r="F11" s="1">
-        <v>479.036</v>
+        <v>501.46620000000001</v>
       </c>
       <c r="G11" s="1">
-        <v>479.03590000000003</v>
+        <v>501.46609999999998</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>0.999999791247422</v>
+        <v>0.99999980058476512</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="2"/>
-        <v>479036</v>
+        <v>501466.2</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="1"/>
-        <v>479035.9</v>
+        <v>501466.1</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
@@ -704,25 +704,25 @@
         <v>17</v>
       </c>
       <c r="E12">
-        <v>10016</v>
+        <v>10015</v>
       </c>
       <c r="F12" s="1">
-        <v>477.907348242811</v>
+        <v>513.82855716425297</v>
       </c>
       <c r="G12" s="1">
-        <v>477.90634984025502</v>
+        <v>513.82835746380397</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999791088678658</v>
+        <v>0.99999961134809223</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="2"/>
-        <v>477907.34824281099</v>
+        <v>513828.55716425297</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="1"/>
-        <v>477906.34984025505</v>
+        <v>513828.35746380396</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
@@ -730,25 +730,25 @@
         <v>19</v>
       </c>
       <c r="E13">
-        <v>10046</v>
+        <v>10032</v>
       </c>
       <c r="F13" s="1">
-        <v>479.30708739796898</v>
+        <v>486.33034290271098</v>
       </c>
       <c r="G13" s="1">
-        <v>479.30688831375602</v>
+        <v>486.32964513556601</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999958464162497</v>
+        <v>0.99999856524036557</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="2"/>
-        <v>479307.08739796898</v>
+        <v>486330.34290271101</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="1"/>
-        <v>479306.88831375603</v>
+        <v>486329.64513556601</v>
       </c>
     </row>
     <row r="14" spans="4:10" x14ac:dyDescent="0.25">
@@ -756,25 +756,25 @@
         <v>26</v>
       </c>
       <c r="E14">
-        <v>10516</v>
+        <v>10485</v>
       </c>
       <c r="F14" s="1">
-        <v>454.49153670597099</v>
+        <v>478.57329518359501</v>
       </c>
       <c r="G14" s="1">
-        <v>454.49144161278002</v>
+        <v>478.57319980925098</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14" si="3">G14/F14</f>
-        <v>0.99999979077016121</v>
-      </c>
-      <c r="I14" s="6">
+        <v>0.99999980071110317</v>
+      </c>
+      <c r="I14" s="7">
         <f t="shared" ref="I14" si="4">F14*1000</f>
-        <v>454491.536705971</v>
-      </c>
-      <c r="J14" s="6">
+        <v>478573.29518359498</v>
+      </c>
+      <c r="J14" s="7">
         <f t="shared" ref="J14" si="5">G14*1000</f>
-        <v>454491.44161278004</v>
+        <v>478573.199809251</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.25">
@@ -790,6 +790,8 @@
       <c r="D16" t="s">
         <v>24</v>
       </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
@@ -807,10 +809,10 @@
       <c r="H17" t="s">
         <v>5</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -822,22 +824,22 @@
         <v>10000</v>
       </c>
       <c r="F18" s="1">
-        <v>155.8672</v>
+        <v>156.1653</v>
       </c>
       <c r="G18" s="1">
-        <v>155.8578</v>
+        <v>156.14869999999999</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" ref="H18:H25" si="6">G18/F18</f>
-        <v>0.99993969225083923</v>
+        <v>0.99989370237818509</v>
       </c>
       <c r="I18" s="7">
         <f>F18*1000</f>
-        <v>155867.19999999998</v>
+        <v>156165.29999999999</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" ref="J18:J25" si="7">G18*1000</f>
-        <v>155857.79999999999</v>
+        <v>156148.69999999998</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
@@ -845,25 +847,25 @@
         <v>14</v>
       </c>
       <c r="E19">
-        <v>10000</v>
+        <v>10015</v>
       </c>
       <c r="F19" s="1">
-        <v>155.7311</v>
+        <v>154.331003494757</v>
       </c>
       <c r="G19" s="1">
-        <v>155.73089999999999</v>
+        <v>154.30064902646001</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="6"/>
-        <v>0.99999871573500732</v>
+        <v>0.99980331581075976</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" ref="I19:I25" si="8">F19*1000</f>
-        <v>155731.1</v>
+        <v>154331.00349475699</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="7"/>
-        <v>155730.9</v>
+        <v>154300.64902646001</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
@@ -874,22 +876,22 @@
         <v>10000</v>
       </c>
       <c r="F20" s="1">
-        <v>157.5197</v>
+        <v>159.18289999999999</v>
       </c>
       <c r="G20" s="1">
-        <v>157.5179</v>
+        <v>159.18</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="6"/>
-        <v>0.99998857285787113</v>
+        <v>0.99998178196276122</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="8"/>
-        <v>157519.70000000001</v>
+        <v>159182.9</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="7"/>
-        <v>157517.9</v>
+        <v>159180</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
@@ -897,25 +899,25 @@
         <v>16</v>
       </c>
       <c r="E21">
-        <v>10031</v>
+        <v>10000</v>
       </c>
       <c r="F21" s="1">
-        <v>160.064599740803</v>
+        <v>159.06950000000001</v>
       </c>
       <c r="G21" s="1">
-        <v>160.03977669225401</v>
+        <v>159.0635</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="6"/>
-        <v>0.99984491856044877</v>
-      </c>
-      <c r="I21" s="5">
+        <v>0.99996228063833736</v>
+      </c>
+      <c r="I21" s="7">
         <f t="shared" si="8"/>
-        <v>160064.59974080301</v>
-      </c>
-      <c r="J21" s="5">
+        <v>159069.5</v>
+      </c>
+      <c r="J21" s="7">
         <f t="shared" si="7"/>
-        <v>160039.776692254</v>
+        <v>159063.5</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
@@ -923,25 +925,25 @@
         <v>18</v>
       </c>
       <c r="E22">
-        <v>10031</v>
+        <v>10016</v>
       </c>
       <c r="F22" s="1">
-        <v>158.68407935400199</v>
+        <v>157.80391373801899</v>
       </c>
       <c r="G22" s="1">
-        <v>158.664041471438</v>
+        <v>157.803414536741</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="6"/>
-        <v>0.99987372468211322</v>
+        <v>0.99999683657226135</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="8"/>
-        <v>158684.07935400199</v>
+        <v>157803.91373801898</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="7"/>
-        <v>158664.04147143799</v>
+        <v>157803.41453674101</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
@@ -949,25 +951,25 @@
         <v>17</v>
       </c>
       <c r="E23">
-        <v>10047</v>
+        <v>10000</v>
       </c>
       <c r="F23" s="1">
-        <v>157.733452771971</v>
+        <v>157.0668</v>
       </c>
       <c r="G23" s="1">
-        <v>157.706877674927</v>
+        <v>157.04249999999999</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="6"/>
-        <v>0.99983151895443245</v>
+        <v>0.99984528875612155</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" si="8"/>
-        <v>157733.452771971</v>
+        <v>157066.79999999999</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="7"/>
-        <v>157706.877674927</v>
+        <v>157042.5</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
@@ -975,25 +977,25 @@
         <v>19</v>
       </c>
       <c r="E24">
-        <v>10656</v>
+        <v>10344</v>
       </c>
       <c r="F24" s="1">
-        <v>155.115709459459</v>
+        <v>154.74013921113601</v>
       </c>
       <c r="G24" s="1">
-        <v>155.09168543543501</v>
+        <v>154.71036349574601</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="6"/>
-        <v>0.9998451219150678</v>
+        <v>0.99980757600748071</v>
       </c>
       <c r="I24" s="7">
         <f t="shared" si="8"/>
-        <v>155115.709459459</v>
+        <v>154740.139211136</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="7"/>
-        <v>155091.68543543501</v>
+        <v>154710.36349574602</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
@@ -1001,25 +1003,25 @@
         <v>26</v>
       </c>
       <c r="E25">
-        <v>13984</v>
+        <v>14766</v>
       </c>
       <c r="F25" s="1">
-        <v>144.775886727688</v>
+        <v>145.95022348638699</v>
       </c>
       <c r="G25" s="1">
-        <v>144.77338386727601</v>
+        <v>145.931125558715</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="6"/>
-        <v>0.99998271217349399</v>
-      </c>
-      <c r="I25" s="6">
+        <v>0.99986914766407486</v>
+      </c>
+      <c r="I25" s="7">
         <f t="shared" si="8"/>
-        <v>144775.88672768799</v>
-      </c>
-      <c r="J25" s="6">
+        <v>145950.223486387</v>
+      </c>
+      <c r="J25" s="7">
         <f t="shared" si="7"/>
-        <v>144773.38386727602</v>
+        <v>145931.12555871499</v>
       </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">
@@ -1035,6 +1037,8 @@
       <c r="D27" t="s">
         <v>23</v>
       </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
@@ -1052,10 +1056,10 @@
       <c r="H28" t="s">
         <v>5</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1064,25 +1068,25 @@
         <v>13</v>
       </c>
       <c r="E29">
-        <v>10750</v>
+        <v>10016</v>
       </c>
       <c r="F29" s="1">
-        <v>354.22995348837202</v>
+        <v>643.02765575079798</v>
       </c>
       <c r="G29" s="1">
-        <v>109.29153488372</v>
+        <v>642.71156150159698</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" ref="H29:H36" si="9">G29/F29</f>
-        <v>0.30853273080789206</v>
-      </c>
-      <c r="I29" s="6">
+        <v>0.99950842822019537</v>
+      </c>
+      <c r="I29" s="7">
         <f>F29*1000</f>
-        <v>354229.95348837203</v>
-      </c>
-      <c r="J29" s="6">
+        <v>643027.65575079795</v>
+      </c>
+      <c r="J29" s="7">
         <f t="shared" ref="J29:J47" si="10">G29*1000</f>
-        <v>109291.53488372</v>
+        <v>642711.56150159694</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
@@ -1090,25 +1094,25 @@
         <v>14</v>
       </c>
       <c r="E30">
-        <v>10734</v>
+        <v>10000</v>
       </c>
       <c r="F30" s="1">
-        <v>462.57918762809697</v>
+        <v>623.25009999999997</v>
       </c>
       <c r="G30" s="1">
-        <v>348.44223961244597</v>
+        <v>622.89980000000003</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="9"/>
-        <v>0.75325965571236531</v>
-      </c>
-      <c r="I30" s="5">
+        <v>0.99943794633967975</v>
+      </c>
+      <c r="I30" s="7">
         <f t="shared" ref="I30:I36" si="11">F30*1000</f>
-        <v>462579.18762809696</v>
-      </c>
-      <c r="J30" s="5">
+        <v>623250.1</v>
+      </c>
+      <c r="J30" s="7">
         <f t="shared" si="10"/>
-        <v>348442.23961244599</v>
+        <v>622899.80000000005</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
@@ -1116,25 +1120,25 @@
         <v>15</v>
       </c>
       <c r="E31">
-        <v>11188</v>
+        <v>10000</v>
       </c>
       <c r="F31" s="1">
-        <v>386.62102252413302</v>
+        <v>619.86180000000002</v>
       </c>
       <c r="G31" s="1">
-        <v>226.291204862352</v>
+        <v>619.50059999999996</v>
       </c>
       <c r="H31" s="4">
         <f t="shared" si="9"/>
-        <v>0.58530496708369451</v>
+        <v>0.9994172894667811</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="11"/>
-        <v>386621.02252413303</v>
+        <v>619861.80000000005</v>
       </c>
       <c r="J31" s="7">
         <f t="shared" si="10"/>
-        <v>226291.20486235199</v>
+        <v>619500.6</v>
       </c>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.25">
@@ -1142,25 +1146,25 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>10844</v>
+        <v>10000</v>
       </c>
       <c r="F32" s="1">
-        <v>396.51346366654298</v>
+        <v>626.26700000000005</v>
       </c>
       <c r="G32" s="1">
-        <v>256.38150129103599</v>
+        <v>625.88969999999995</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="9"/>
-        <v>0.64658964898767179</v>
+        <v>0.99939754130426783</v>
       </c>
       <c r="I32" s="7">
         <f t="shared" si="11"/>
-        <v>396513.46366654296</v>
+        <v>626267</v>
       </c>
       <c r="J32" s="7">
         <f t="shared" si="10"/>
-        <v>256381.50129103599</v>
+        <v>625889.69999999995</v>
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.25">
@@ -1168,25 +1172,25 @@
         <v>18</v>
       </c>
       <c r="E33">
-        <v>10735</v>
+        <v>10000</v>
       </c>
       <c r="F33" s="1">
-        <v>400.01686073590997</v>
+        <v>618.21450000000004</v>
       </c>
       <c r="G33" s="1">
-        <v>265.43027480204898</v>
+        <v>617.83079999999995</v>
       </c>
       <c r="H33" s="4">
         <f t="shared" si="9"/>
-        <v>0.66354771724806205</v>
+        <v>0.99937934163627662</v>
       </c>
       <c r="I33" s="7">
         <f t="shared" si="11"/>
-        <v>400016.86073590996</v>
+        <v>618214.5</v>
       </c>
       <c r="J33" s="7">
         <f t="shared" si="10"/>
-        <v>265430.27480204898</v>
+        <v>617830.79999999993</v>
       </c>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.25">
@@ -1194,25 +1198,25 @@
         <v>17</v>
       </c>
       <c r="E34">
-        <v>10281</v>
+        <v>10000</v>
       </c>
       <c r="F34" s="1">
-        <v>418.87686022760403</v>
+        <v>619.77620000000002</v>
       </c>
       <c r="G34" s="1">
-        <v>267.55587977823097</v>
+        <v>619.41129999999998</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="9"/>
-        <v>0.63874590645291274</v>
+        <v>0.9994112390892067</v>
       </c>
       <c r="I34" s="7">
         <f t="shared" si="11"/>
-        <v>418876.86022760405</v>
+        <v>619776.20000000007</v>
       </c>
       <c r="J34" s="7">
         <f t="shared" si="10"/>
-        <v>267555.87977823097</v>
+        <v>619411.29999999993</v>
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.25">
@@ -1220,25 +1224,25 @@
         <v>19</v>
       </c>
       <c r="E35">
-        <v>10578</v>
+        <v>10031</v>
       </c>
       <c r="F35" s="1">
-        <v>400.64501796180701</v>
+        <v>639.89552387598405</v>
       </c>
       <c r="G35" s="1">
-        <v>264.66921913405099</v>
+        <v>639.47732030704799</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="9"/>
-        <v>0.66060778811252208</v>
+        <v>0.9993464502354964</v>
       </c>
       <c r="I35" s="7">
         <f t="shared" si="11"/>
-        <v>400645.01796180703</v>
+        <v>639895.52387598401</v>
       </c>
       <c r="J35" s="7">
         <f t="shared" si="10"/>
-        <v>264669.219134051</v>
+        <v>639477.32030704804</v>
       </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.25">
@@ -1246,25 +1250,25 @@
         <v>26</v>
       </c>
       <c r="E36">
-        <v>11422</v>
+        <v>10422</v>
       </c>
       <c r="F36" s="1">
-        <v>409.34468569427401</v>
+        <v>635.17232776818196</v>
       </c>
       <c r="G36" s="1">
-        <v>291.22666783400399</v>
+        <v>634.59719823450303</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="9"/>
-        <v>0.71144606980805303</v>
+        <v>0.99909452992749259</v>
       </c>
       <c r="I36" s="7">
         <f t="shared" si="11"/>
-        <v>409344.68569427403</v>
+        <v>635172.32776818192</v>
       </c>
       <c r="J36" s="7">
         <f t="shared" si="10"/>
-        <v>291226.66783400398</v>
+        <v>634597.19823450304</v>
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.25">
@@ -1311,25 +1315,25 @@
         <v>13</v>
       </c>
       <c r="E40">
-        <v>11844</v>
+        <v>10000</v>
       </c>
       <c r="F40" s="1">
-        <v>385.048463356973</v>
+        <v>240.5558</v>
       </c>
       <c r="G40" s="1">
-        <v>45.845997973657497</v>
+        <v>240.18809999999999</v>
       </c>
       <c r="H40" s="4">
         <f t="shared" ref="H40:H47" si="12">G40/F40</f>
-        <v>0.11906552638584177</v>
+        <v>0.99847145651861224</v>
       </c>
       <c r="I40" s="7">
         <f>F40*1000</f>
-        <v>385048.46335697302</v>
+        <v>240555.80000000002</v>
       </c>
       <c r="J40" s="7">
         <f t="shared" ref="J40:J47" si="13">G40*1000</f>
-        <v>45845.997973657497</v>
+        <v>240188.1</v>
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.25">
@@ -1337,25 +1341,25 @@
         <v>14</v>
       </c>
       <c r="E41">
-        <v>11078</v>
+        <v>10000</v>
       </c>
       <c r="F41" s="1">
-        <v>431.89646145513598</v>
+        <v>243.40350000000001</v>
       </c>
       <c r="G41" s="1">
-        <v>74.857465246434302</v>
+        <v>243.018</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" si="12"/>
-        <v>0.17332271024917914</v>
+        <v>0.99841621012023241</v>
       </c>
       <c r="I41" s="7">
         <f t="shared" ref="I41:I47" si="14">F41*1000</f>
-        <v>431896.46145513596</v>
-      </c>
-      <c r="J41" s="5">
+        <v>243403.5</v>
+      </c>
+      <c r="J41" s="7">
         <f t="shared" si="13"/>
-        <v>74857.465246434309</v>
+        <v>243018</v>
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.25">
@@ -1366,22 +1370,22 @@
         <v>10000</v>
       </c>
       <c r="F42" s="1">
-        <v>484.9076</v>
+        <v>245.88810000000001</v>
       </c>
       <c r="G42" s="1">
-        <v>41.087600000000002</v>
+        <v>245.50700000000001</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" si="12"/>
-        <v>8.4732843948001638E-2</v>
-      </c>
-      <c r="I42" s="5">
+        <v>0.99845010799627965</v>
+      </c>
+      <c r="I42" s="7">
         <f t="shared" si="14"/>
-        <v>484907.6</v>
+        <v>245888.1</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="13"/>
-        <v>41087.599999999999</v>
+        <v>245507</v>
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.25">
@@ -1389,25 +1393,25 @@
         <v>16</v>
       </c>
       <c r="E43">
-        <v>11797</v>
+        <v>10000</v>
       </c>
       <c r="F43" s="1">
-        <v>395.90590828176602</v>
+        <v>242.40180000000001</v>
       </c>
       <c r="G43" s="1">
-        <v>38.022039501568102</v>
+        <v>242.006</v>
       </c>
       <c r="H43" s="4">
         <f t="shared" si="12"/>
-        <v>9.6038070425834204E-2</v>
+        <v>0.99836717384111828</v>
       </c>
       <c r="I43" s="7">
         <f t="shared" si="14"/>
-        <v>395905.90828176599</v>
+        <v>242401.80000000002</v>
       </c>
       <c r="J43" s="7">
         <f t="shared" si="13"/>
-        <v>38022.039501568099</v>
+        <v>242006</v>
       </c>
     </row>
     <row r="44" spans="4:10" x14ac:dyDescent="0.25">
@@ -1415,25 +1419,25 @@
         <v>18</v>
       </c>
       <c r="E44">
-        <v>10578</v>
+        <v>10031</v>
       </c>
       <c r="F44" s="1">
-        <v>451.197012667801</v>
+        <v>243.67879573322699</v>
       </c>
       <c r="G44" s="1">
-        <v>46.063433541312101</v>
+        <v>243.30824444222901</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="12"/>
-        <v>0.10209161906669545</v>
+        <v>0.99847934536165528</v>
       </c>
       <c r="I44" s="7">
         <f t="shared" si="14"/>
-        <v>451197.012667801</v>
+        <v>243678.79573322699</v>
       </c>
       <c r="J44" s="7">
         <f t="shared" si="13"/>
-        <v>46063.433541312101</v>
+        <v>243308.24444222901</v>
       </c>
     </row>
     <row r="45" spans="4:10" x14ac:dyDescent="0.25">
@@ -1444,22 +1448,22 @@
         <v>10047</v>
       </c>
       <c r="F45" s="1">
-        <v>467.237881954812</v>
+        <v>242.50900766397899</v>
       </c>
       <c r="G45" s="1">
-        <v>44.563551308848403</v>
+        <v>242.10759430675799</v>
       </c>
       <c r="H45" s="4">
         <f t="shared" si="12"/>
-        <v>9.5376580174546463E-2</v>
+        <v>0.99834474867103817</v>
       </c>
       <c r="I45" s="7">
         <f t="shared" si="14"/>
-        <v>467237.88195481198</v>
+        <v>242509.00766397899</v>
       </c>
       <c r="J45" s="7">
         <f t="shared" si="13"/>
-        <v>44563.5513088484</v>
+        <v>242107.59430675799</v>
       </c>
     </row>
     <row r="46" spans="4:10" x14ac:dyDescent="0.25">
@@ -1467,25 +1471,25 @@
         <v>19</v>
       </c>
       <c r="E46">
-        <v>10985</v>
+        <v>10266</v>
       </c>
       <c r="F46" s="1">
-        <v>426.72389622212103</v>
+        <v>240.66043249561599</v>
       </c>
       <c r="G46" s="1">
-        <v>49.6939462903959</v>
+        <v>240.292518994739</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="12"/>
-        <v>0.11645456636093539</v>
+        <v>0.99847123394127657</v>
       </c>
       <c r="I46" s="7">
         <f t="shared" si="14"/>
-        <v>426723.89622212102</v>
+        <v>240660.432495616</v>
       </c>
       <c r="J46" s="7">
         <f t="shared" si="13"/>
-        <v>49693.946290395899</v>
+        <v>240292.51899473899</v>
       </c>
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.25">
@@ -1493,25 +1497,25 @@
         <v>26</v>
       </c>
       <c r="E47">
-        <v>28281</v>
+        <v>12141</v>
       </c>
       <c r="F47" s="1">
-        <v>176.53824122202099</v>
+        <v>226.40466188946499</v>
       </c>
       <c r="G47" s="1">
-        <v>23.4388812276793</v>
+        <v>225.919034675891</v>
       </c>
       <c r="H47" s="4">
         <f t="shared" si="12"/>
-        <v>0.13276942754970408</v>
-      </c>
-      <c r="I47" s="6">
+        <v>0.99785504764115196</v>
+      </c>
+      <c r="I47" s="7">
         <f t="shared" si="14"/>
-        <v>176538.241222021</v>
-      </c>
-      <c r="J47" s="6">
+        <v>226404.661889465</v>
+      </c>
+      <c r="J47" s="7">
         <f t="shared" si="13"/>
-        <v>23438.8812276793</v>
+        <v>225919.03467589099</v>
       </c>
     </row>
     <row r="48" spans="4:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajustes al procesador para rechazar sólo threads externos
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120704/Performance del procesador.xlsx
+++ b/Documentacion/drafts/20120704/Performance del procesador.xlsx
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,25 +574,25 @@
         <v>13</v>
       </c>
       <c r="E7">
-        <v>10016</v>
+        <v>10000</v>
       </c>
       <c r="F7" s="1">
-        <v>526.24940095846603</v>
+        <v>505.27679999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>526.24790335463194</v>
+        <v>505.27659999999997</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" ref="H7:H13" si="0">G7/F7</f>
-        <v>0.99999715419375046</v>
-      </c>
-      <c r="I7" s="7">
+        <v>0.9999996041773539</v>
+      </c>
+      <c r="I7" s="5">
         <f>F7*1000</f>
-        <v>526249.40095846599</v>
-      </c>
-      <c r="J7" s="7">
+        <v>505276.8</v>
+      </c>
+      <c r="J7" s="5">
         <f t="shared" ref="J7:J50" si="1">G7*1000</f>
-        <v>526247.90335463197</v>
+        <v>505276.6</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
@@ -603,22 +603,22 @@
         <v>10000</v>
       </c>
       <c r="F8" s="1">
-        <v>476.42959999999999</v>
+        <v>498.1447</v>
       </c>
       <c r="G8" s="1">
-        <v>476.42910000000001</v>
+        <v>498.14449999999999</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999895052700338</v>
+        <v>0.99999959851023201</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" ref="I8:I13" si="2">F8*1000</f>
-        <v>476429.6</v>
+        <v>498144.7</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="1"/>
-        <v>476429.1</v>
+        <v>498144.5</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
@@ -629,22 +629,22 @@
         <v>10000</v>
       </c>
       <c r="F9" s="1">
-        <v>460.37329999999997</v>
+        <v>480.28219999999999</v>
       </c>
       <c r="G9" s="1">
-        <v>460.3732</v>
+        <v>480.28219999999999</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999978278497037</v>
+        <v>1</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="2"/>
-        <v>460373.3</v>
+        <v>480282.2</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>460373.2</v>
+        <v>480282.2</v>
       </c>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.25">
@@ -652,25 +652,25 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>10016</v>
+        <v>10000</v>
       </c>
       <c r="F10" s="1">
-        <v>487.64327076677301</v>
+        <v>476.56889999999999</v>
       </c>
       <c r="G10" s="1">
-        <v>487.64327076677301</v>
+        <v>476.56700000000001</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I10" s="7">
+        <v>0.99999601316829534</v>
+      </c>
+      <c r="I10" s="6">
         <f t="shared" si="2"/>
-        <v>487643.27076677303</v>
-      </c>
-      <c r="J10" s="7">
+        <v>476568.89999999997</v>
+      </c>
+      <c r="J10" s="6">
         <f t="shared" si="1"/>
-        <v>487643.27076677303</v>
+        <v>476567</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
@@ -678,25 +678,25 @@
         <v>18</v>
       </c>
       <c r="E11">
-        <v>10000</v>
+        <v>10015</v>
       </c>
       <c r="F11" s="1">
-        <v>501.46620000000001</v>
+        <v>491.16015976035902</v>
       </c>
       <c r="G11" s="1">
-        <v>501.46609999999998</v>
+        <v>491.15996005991002</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999980058476512</v>
+        <v>0.99999959341073363</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="2"/>
-        <v>501466.2</v>
+        <v>491160.15976035903</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="1"/>
-        <v>501466.1</v>
+        <v>491159.96005991002</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
@@ -704,25 +704,25 @@
         <v>17</v>
       </c>
       <c r="E12">
-        <v>10015</v>
+        <v>10000</v>
       </c>
       <c r="F12" s="1">
-        <v>513.82855716425297</v>
+        <v>497.45499999999998</v>
       </c>
       <c r="G12" s="1">
-        <v>513.82835746380397</v>
+        <v>497.45490000000001</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999961134809223</v>
+        <v>0.99999979897679192</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="2"/>
-        <v>513828.55716425297</v>
+        <v>497455</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="1"/>
-        <v>513828.35746380396</v>
+        <v>497454.9</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
@@ -730,25 +730,25 @@
         <v>19</v>
       </c>
       <c r="E13">
-        <v>10032</v>
+        <v>10047</v>
       </c>
       <c r="F13" s="1">
-        <v>486.33034290271098</v>
+        <v>482.168707076739</v>
       </c>
       <c r="G13" s="1">
-        <v>486.32964513556601</v>
+        <v>482.16860754454001</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999856524036557</v>
+        <v>0.999999793573914</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="2"/>
-        <v>486330.34290271101</v>
+        <v>482168.707076739</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="1"/>
-        <v>486329.64513556601</v>
+        <v>482168.60754454002</v>
       </c>
     </row>
     <row r="14" spans="4:10" x14ac:dyDescent="0.25">
@@ -759,22 +759,22 @@
         <v>10485</v>
       </c>
       <c r="F14" s="1">
-        <v>478.57329518359501</v>
+        <v>479.17672865998998</v>
       </c>
       <c r="G14" s="1">
-        <v>478.57319980925098</v>
+        <v>479.17663328564601</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14" si="3">G14/F14</f>
-        <v>0.99999980071110317</v>
+        <v>0.99999980096207042</v>
       </c>
       <c r="I14" s="7">
         <f t="shared" ref="I14" si="4">F14*1000</f>
-        <v>478573.29518359498</v>
+        <v>479176.72865998995</v>
       </c>
       <c r="J14" s="7">
         <f t="shared" ref="J14" si="5">G14*1000</f>
-        <v>478573.199809251</v>
+        <v>479176.63328564598</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.25">
@@ -821,25 +821,25 @@
         <v>13</v>
       </c>
       <c r="E18">
-        <v>10000</v>
+        <v>10016</v>
       </c>
       <c r="F18" s="1">
-        <v>156.1653</v>
+        <v>154.349440894568</v>
       </c>
       <c r="G18" s="1">
-        <v>156.14869999999999</v>
+        <v>154.34345047923301</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" ref="H18:H25" si="6">G18/F18</f>
-        <v>0.99989370237818509</v>
+        <v>0.99996118926443611</v>
       </c>
       <c r="I18" s="7">
         <f>F18*1000</f>
-        <v>156165.29999999999</v>
+        <v>154349.44089456802</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" ref="J18:J25" si="7">G18*1000</f>
-        <v>156148.69999999998</v>
+        <v>154343.45047923303</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
@@ -847,25 +847,25 @@
         <v>14</v>
       </c>
       <c r="E19">
-        <v>10015</v>
+        <v>10000</v>
       </c>
       <c r="F19" s="1">
-        <v>154.331003494757</v>
+        <v>157.9479</v>
       </c>
       <c r="G19" s="1">
-        <v>154.30064902646001</v>
+        <v>157.94759999999999</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="6"/>
-        <v>0.99980331581075976</v>
+        <v>0.99999810063951466</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" ref="I19:I25" si="8">F19*1000</f>
-        <v>154331.00349475699</v>
+        <v>157947.9</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="7"/>
-        <v>154300.64902646001</v>
+        <v>157947.6</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
@@ -876,22 +876,22 @@
         <v>10000</v>
       </c>
       <c r="F20" s="1">
-        <v>159.18289999999999</v>
+        <v>154.94900000000001</v>
       </c>
       <c r="G20" s="1">
-        <v>159.18</v>
+        <v>154.9282</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="6"/>
-        <v>0.99998178196276122</v>
+        <v>0.99986576228307378</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="8"/>
-        <v>159182.9</v>
+        <v>154949</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="7"/>
-        <v>159180</v>
+        <v>154928.20000000001</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
@@ -902,22 +902,22 @@
         <v>10000</v>
       </c>
       <c r="F21" s="1">
-        <v>159.06950000000001</v>
+        <v>158.68170000000001</v>
       </c>
       <c r="G21" s="1">
-        <v>159.0635</v>
+        <v>158.6765</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="6"/>
-        <v>0.99996228063833736</v>
-      </c>
-      <c r="I21" s="7">
+        <v>0.99996722999564536</v>
+      </c>
+      <c r="I21" s="5">
         <f t="shared" si="8"/>
-        <v>159069.5</v>
-      </c>
-      <c r="J21" s="7">
+        <v>158681.70000000001</v>
+      </c>
+      <c r="J21" s="5">
         <f t="shared" si="7"/>
-        <v>159063.5</v>
+        <v>158676.5</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
@@ -928,22 +928,22 @@
         <v>10016</v>
       </c>
       <c r="F22" s="1">
-        <v>157.80391373801899</v>
+        <v>155.939197284345</v>
       </c>
       <c r="G22" s="1">
-        <v>157.803414536741</v>
+        <v>155.931409744408</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="6"/>
-        <v>0.99999683657226135</v>
+        <v>0.99995006040769341</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="8"/>
-        <v>157803.91373801898</v>
+        <v>155939.19728434499</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="7"/>
-        <v>157803.41453674101</v>
+        <v>155931.40974440801</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
@@ -951,25 +951,25 @@
         <v>17</v>
       </c>
       <c r="E23">
-        <v>10000</v>
+        <v>10047</v>
       </c>
       <c r="F23" s="1">
-        <v>157.0668</v>
+        <v>158.49676520354299</v>
       </c>
       <c r="G23" s="1">
-        <v>157.04249999999999</v>
+        <v>158.49547128495999</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="6"/>
-        <v>0.99984528875612155</v>
+        <v>0.99999183630920585</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" si="8"/>
-        <v>157066.79999999999</v>
+        <v>158496.76520354298</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="7"/>
-        <v>157042.5</v>
+        <v>158495.47128495999</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
@@ -977,25 +977,25 @@
         <v>19</v>
       </c>
       <c r="E24">
-        <v>10344</v>
+        <v>10407</v>
       </c>
       <c r="F24" s="1">
-        <v>154.74013921113601</v>
+        <v>155.35620255597101</v>
       </c>
       <c r="G24" s="1">
-        <v>154.71036349574601</v>
+        <v>155.32708753723401</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="6"/>
-        <v>0.99980757600748071</v>
+        <v>0.99981259184855198</v>
       </c>
       <c r="I24" s="7">
         <f t="shared" si="8"/>
-        <v>154740.139211136</v>
+        <v>155356.20255597102</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="7"/>
-        <v>154710.36349574602</v>
+        <v>155327.08753723401</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
@@ -1003,25 +1003,25 @@
         <v>26</v>
       </c>
       <c r="E25">
-        <v>14766</v>
+        <v>15156</v>
       </c>
       <c r="F25" s="1">
-        <v>145.95022348638699</v>
+        <v>143.80238849300599</v>
       </c>
       <c r="G25" s="1">
-        <v>145.931125558715</v>
+        <v>143.785629453681</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="6"/>
-        <v>0.99986914766407486</v>
-      </c>
-      <c r="I25" s="7">
+        <v>0.9998834578514264</v>
+      </c>
+      <c r="I25" s="6">
         <f t="shared" si="8"/>
-        <v>145950.223486387</v>
-      </c>
-      <c r="J25" s="7">
+        <v>143802.388493006</v>
+      </c>
+      <c r="J25" s="6">
         <f t="shared" si="7"/>
-        <v>145931.12555871499</v>
+        <v>143785.629453681</v>
       </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">
@@ -1068,25 +1068,25 @@
         <v>13</v>
       </c>
       <c r="E29">
-        <v>10016</v>
+        <v>10000</v>
       </c>
       <c r="F29" s="1">
-        <v>643.02765575079798</v>
+        <v>637.05709999999999</v>
       </c>
       <c r="G29" s="1">
-        <v>642.71156150159698</v>
+        <v>636.75990000000002</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" ref="H29:H36" si="9">G29/F29</f>
-        <v>0.99950842822019537</v>
-      </c>
-      <c r="I29" s="7">
+        <v>0.9995334798089528</v>
+      </c>
+      <c r="I29" s="5">
         <f>F29*1000</f>
-        <v>643027.65575079795</v>
-      </c>
-      <c r="J29" s="7">
+        <v>637057.1</v>
+      </c>
+      <c r="J29" s="5">
         <f t="shared" ref="J29:J47" si="10">G29*1000</f>
-        <v>642711.56150159694</v>
+        <v>636759.9</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
@@ -1097,22 +1097,22 @@
         <v>10000</v>
       </c>
       <c r="F30" s="1">
-        <v>623.25009999999997</v>
+        <v>605.03750000000002</v>
       </c>
       <c r="G30" s="1">
-        <v>622.89980000000003</v>
+        <v>604.69970000000001</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="9"/>
-        <v>0.99943794633967975</v>
-      </c>
-      <c r="I30" s="7">
+        <v>0.99944168749870876</v>
+      </c>
+      <c r="I30" s="6">
         <f t="shared" ref="I30:I36" si="11">F30*1000</f>
-        <v>623250.1</v>
-      </c>
-      <c r="J30" s="7">
+        <v>605037.5</v>
+      </c>
+      <c r="J30" s="6">
         <f t="shared" si="10"/>
-        <v>622899.80000000005</v>
+        <v>604699.69999999995</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
@@ -1123,22 +1123,22 @@
         <v>10000</v>
       </c>
       <c r="F31" s="1">
-        <v>619.86180000000002</v>
+        <v>606.27499999999998</v>
       </c>
       <c r="G31" s="1">
-        <v>619.50059999999996</v>
+        <v>605.9117</v>
       </c>
       <c r="H31" s="4">
         <f t="shared" si="9"/>
-        <v>0.9994172894667811</v>
+        <v>0.9994007669786813</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="11"/>
-        <v>619861.80000000005</v>
+        <v>606275</v>
       </c>
       <c r="J31" s="7">
         <f t="shared" si="10"/>
-        <v>619500.6</v>
+        <v>605911.69999999995</v>
       </c>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.25">
@@ -1149,22 +1149,22 @@
         <v>10000</v>
       </c>
       <c r="F32" s="1">
-        <v>626.26700000000005</v>
+        <v>608.83600000000001</v>
       </c>
       <c r="G32" s="1">
-        <v>625.88969999999995</v>
+        <v>608.46579999999994</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="9"/>
-        <v>0.99939754130426783</v>
+        <v>0.99939195448363749</v>
       </c>
       <c r="I32" s="7">
         <f t="shared" si="11"/>
-        <v>626267</v>
+        <v>608836</v>
       </c>
       <c r="J32" s="7">
         <f t="shared" si="10"/>
-        <v>625889.69999999995</v>
+        <v>608465.79999999993</v>
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.25">
@@ -1175,22 +1175,22 @@
         <v>10000</v>
       </c>
       <c r="F33" s="1">
-        <v>618.21450000000004</v>
+        <v>607.4579</v>
       </c>
       <c r="G33" s="1">
-        <v>617.83079999999995</v>
+        <v>607.07770000000005</v>
       </c>
       <c r="H33" s="4">
         <f t="shared" si="9"/>
-        <v>0.99937934163627662</v>
+        <v>0.99937411300437451</v>
       </c>
       <c r="I33" s="7">
         <f t="shared" si="11"/>
-        <v>618214.5</v>
+        <v>607457.9</v>
       </c>
       <c r="J33" s="7">
         <f t="shared" si="10"/>
-        <v>617830.79999999993</v>
+        <v>607077.70000000007</v>
       </c>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.25">
@@ -1198,25 +1198,25 @@
         <v>17</v>
       </c>
       <c r="E34">
-        <v>10000</v>
+        <v>10015</v>
       </c>
       <c r="F34" s="1">
-        <v>619.77620000000002</v>
+        <v>605.889465801298</v>
       </c>
       <c r="G34" s="1">
-        <v>619.41129999999998</v>
+        <v>605.500848726909</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="9"/>
-        <v>0.9994112390892067</v>
+        <v>0.99935860070801019</v>
       </c>
       <c r="I34" s="7">
         <f t="shared" si="11"/>
-        <v>619776.20000000007</v>
+        <v>605889.46580129804</v>
       </c>
       <c r="J34" s="7">
         <f t="shared" si="10"/>
-        <v>619411.29999999993</v>
+        <v>605500.84872690903</v>
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.25">
@@ -1227,22 +1227,22 @@
         <v>10031</v>
       </c>
       <c r="F35" s="1">
-        <v>639.89552387598405</v>
+        <v>634.514106270561</v>
       </c>
       <c r="G35" s="1">
-        <v>639.47732030704799</v>
+        <v>634.09550393779205</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="9"/>
-        <v>0.9993464502354964</v>
+        <v>0.99934027891794341</v>
       </c>
       <c r="I35" s="7">
         <f t="shared" si="11"/>
-        <v>639895.52387598401</v>
+        <v>634514.10627056099</v>
       </c>
       <c r="J35" s="7">
         <f t="shared" si="10"/>
-        <v>639477.32030704804</v>
+        <v>634095.50393779203</v>
       </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.25">
@@ -1250,25 +1250,25 @@
         <v>26</v>
       </c>
       <c r="E36">
-        <v>10422</v>
+        <v>10406</v>
       </c>
       <c r="F36" s="1">
-        <v>635.17232776818196</v>
+        <v>632.73861233903494</v>
       </c>
       <c r="G36" s="1">
-        <v>634.59719823450303</v>
+        <v>632.16557755141196</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="9"/>
-        <v>0.99909452992749259</v>
+        <v>0.99909435780202405</v>
       </c>
       <c r="I36" s="7">
         <f t="shared" si="11"/>
-        <v>635172.32776818192</v>
+        <v>632738.61233903491</v>
       </c>
       <c r="J36" s="7">
         <f t="shared" si="10"/>
-        <v>634597.19823450304</v>
+        <v>632165.57755141193</v>
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.25">
@@ -1318,22 +1318,22 @@
         <v>10000</v>
       </c>
       <c r="F40" s="1">
-        <v>240.5558</v>
+        <v>240.32740000000001</v>
       </c>
       <c r="G40" s="1">
-        <v>240.18809999999999</v>
+        <v>239.93090000000001</v>
       </c>
       <c r="H40" s="4">
         <f t="shared" ref="H40:H47" si="12">G40/F40</f>
-        <v>0.99847145651861224</v>
+        <v>0.9983501673134233</v>
       </c>
       <c r="I40" s="7">
         <f>F40*1000</f>
-        <v>240555.80000000002</v>
+        <v>240327.40000000002</v>
       </c>
       <c r="J40" s="7">
         <f t="shared" ref="J40:J47" si="13">G40*1000</f>
-        <v>240188.1</v>
+        <v>239930.9</v>
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.25">
@@ -1344,22 +1344,22 @@
         <v>10000</v>
       </c>
       <c r="F41" s="1">
-        <v>243.40350000000001</v>
+        <v>242.6567</v>
       </c>
       <c r="G41" s="1">
-        <v>243.018</v>
+        <v>242.27330000000001</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" si="12"/>
-        <v>0.99841621012023241</v>
-      </c>
-      <c r="I41" s="7">
+        <v>0.99841999005178927</v>
+      </c>
+      <c r="I41" s="5">
         <f t="shared" ref="I41:I47" si="14">F41*1000</f>
-        <v>243403.5</v>
-      </c>
-      <c r="J41" s="7">
+        <v>242656.7</v>
+      </c>
+      <c r="J41" s="5">
         <f t="shared" si="13"/>
-        <v>243018</v>
+        <v>242273.30000000002</v>
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.25">
@@ -1370,22 +1370,22 @@
         <v>10000</v>
       </c>
       <c r="F42" s="1">
-        <v>245.88810000000001</v>
+        <v>241.17760000000001</v>
       </c>
       <c r="G42" s="1">
-        <v>245.50700000000001</v>
+        <v>240.77709999999999</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" si="12"/>
-        <v>0.99845010799627965</v>
+        <v>0.99833939802037996</v>
       </c>
       <c r="I42" s="7">
         <f t="shared" si="14"/>
-        <v>245888.1</v>
+        <v>241177.60000000001</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="13"/>
-        <v>245507</v>
+        <v>240777.09999999998</v>
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.25">
@@ -1393,25 +1393,25 @@
         <v>16</v>
       </c>
       <c r="E43">
-        <v>10000</v>
+        <v>10015</v>
       </c>
       <c r="F43" s="1">
-        <v>242.40180000000001</v>
+        <v>222.67538691962</v>
       </c>
       <c r="G43" s="1">
-        <v>242.006</v>
+        <v>222.29435846230601</v>
       </c>
       <c r="H43" s="4">
         <f t="shared" si="12"/>
-        <v>0.99836717384111828</v>
+        <v>0.99828886136638206</v>
       </c>
       <c r="I43" s="7">
         <f t="shared" si="14"/>
-        <v>242401.80000000002</v>
+        <v>222675.38691961998</v>
       </c>
       <c r="J43" s="7">
         <f t="shared" si="13"/>
-        <v>242006</v>
+        <v>222294.358462306</v>
       </c>
     </row>
     <row r="44" spans="4:10" x14ac:dyDescent="0.25">
@@ -1419,25 +1419,25 @@
         <v>18</v>
       </c>
       <c r="E44">
-        <v>10031</v>
+        <v>10000</v>
       </c>
       <c r="F44" s="1">
-        <v>243.67879573322699</v>
+        <v>241.75960000000001</v>
       </c>
       <c r="G44" s="1">
-        <v>243.30824444222901</v>
+        <v>241.38130000000001</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="12"/>
-        <v>0.99847934536165528</v>
+        <v>0.99843522242756855</v>
       </c>
       <c r="I44" s="7">
         <f t="shared" si="14"/>
-        <v>243678.79573322699</v>
+        <v>241759.6</v>
       </c>
       <c r="J44" s="7">
         <f t="shared" si="13"/>
-        <v>243308.24444222901</v>
+        <v>241381.30000000002</v>
       </c>
     </row>
     <row r="45" spans="4:10" x14ac:dyDescent="0.25">
@@ -1448,22 +1448,22 @@
         <v>10047</v>
       </c>
       <c r="F45" s="1">
-        <v>242.50900766397899</v>
+        <v>222.124514780531</v>
       </c>
       <c r="G45" s="1">
-        <v>242.10759430675799</v>
+        <v>221.759331143624</v>
       </c>
       <c r="H45" s="4">
         <f t="shared" si="12"/>
-        <v>0.99834474867103817</v>
-      </c>
-      <c r="I45" s="7">
+        <v>0.9983559507726204</v>
+      </c>
+      <c r="I45" s="6">
         <f t="shared" si="14"/>
-        <v>242509.00766397899</v>
-      </c>
-      <c r="J45" s="7">
+        <v>222124.514780531</v>
+      </c>
+      <c r="J45" s="6">
         <f t="shared" si="13"/>
-        <v>242107.59430675799</v>
+        <v>221759.331143624</v>
       </c>
     </row>
     <row r="46" spans="4:10" x14ac:dyDescent="0.25">
@@ -1471,25 +1471,25 @@
         <v>19</v>
       </c>
       <c r="E46">
-        <v>10266</v>
+        <v>10157</v>
       </c>
       <c r="F46" s="1">
-        <v>240.66043249561599</v>
+        <v>237.25558727970801</v>
       </c>
       <c r="G46" s="1">
-        <v>240.292518994739</v>
+        <v>236.841882445604</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="12"/>
-        <v>0.99847123394127657</v>
+        <v>0.99825629044673969</v>
       </c>
       <c r="I46" s="7">
         <f t="shared" si="14"/>
-        <v>240660.432495616</v>
+        <v>237255.58727970801</v>
       </c>
       <c r="J46" s="7">
         <f t="shared" si="13"/>
-        <v>240292.51899473899</v>
+        <v>236841.88244560399</v>
       </c>
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.25">
@@ -1497,25 +1497,25 @@
         <v>26</v>
       </c>
       <c r="E47">
-        <v>12141</v>
+        <v>11453</v>
       </c>
       <c r="F47" s="1">
-        <v>226.40466188946499</v>
+        <v>224.018073867109</v>
       </c>
       <c r="G47" s="1">
-        <v>225.919034675891</v>
+        <v>223.49707500218199</v>
       </c>
       <c r="H47" s="4">
         <f t="shared" si="12"/>
-        <v>0.99785504764115196</v>
+        <v>0.99767429986369727</v>
       </c>
       <c r="I47" s="7">
         <f t="shared" si="14"/>
-        <v>226404.661889465</v>
+        <v>224018.07386710899</v>
       </c>
       <c r="J47" s="7">
         <f t="shared" si="13"/>
-        <v>225919.03467589099</v>
+        <v>223497.07500218198</v>
       </c>
     </row>
     <row r="48" spans="4:10" x14ac:dyDescent="0.25">

</xml_diff>